<commit_message>
Testes de cores usando classes
</commit_message>
<xml_diff>
--- a/Definições de sistema.xlsx
+++ b/Definições de sistema.xlsx
@@ -30,7 +30,6 @@
     <definedName name="modelos">Tabelas!$H$2:$K$5</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="167">
   <si>
     <t xml:space="preserve">Definições do sistema de frotas </t>
   </si>
@@ -273,9 +272,6 @@
     <t>foreignkey da marca de veiculos e componentes</t>
   </si>
   <si>
-    <t>MODELOS DE VEICULOS E COMPONENTES</t>
-  </si>
-  <si>
     <t>viscosidade SAE</t>
   </si>
   <si>
@@ -291,9 +287,6 @@
     <t>pode ser cadastrado item com mais de uma cor</t>
   </si>
   <si>
-    <t>APLICAÇÃO</t>
-  </si>
-  <si>
     <t>eixo</t>
   </si>
   <si>
@@ -535,6 +528,18 @@
   </si>
   <si>
     <t>foreignkey do arquivo de complemento (carroceria, bau, etc) ou sem implemento. Condicional ao equipamento utilizar algum implemento. Como nos anteriores pode haver um registro com nenhum implemento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sim </t>
+  </si>
+  <si>
+    <t>foreignkey da tabela de modelos de veiculos e complementos</t>
+  </si>
+  <si>
+    <t>MODELOS DE VEICULOS E COMPONENTES   ok</t>
+  </si>
+  <si>
+    <t>APLICAÇÃO    ok</t>
   </si>
 </sst>
 </file>
@@ -703,7 +708,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -768,6 +773,7 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="justify" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1055,17 +1061,17 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1073,7 +1079,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1081,7 +1087,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1089,31 +1095,31 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A13" s="42"/>
     </row>
   </sheetData>
@@ -1126,29 +1132,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.31640625" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" customWidth="1"/>
-    <col min="14" max="14" width="20.109375" customWidth="1"/>
-    <col min="20" max="20" width="20.6640625" customWidth="1"/>
-    <col min="26" max="26" width="26.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21.6796875" customWidth="1"/>
+    <col min="14" max="14" width="20.08984375" customWidth="1"/>
+    <col min="20" max="20" width="20.6796875" customWidth="1"/>
+    <col min="26" max="26" width="26.6796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.75">
       <c r="A1" s="43" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.75">
       <c r="A2" s="43"/>
       <c r="B2" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>26</v>
@@ -1158,7 +1164,7 @@
       </c>
       <c r="E2" s="3"/>
       <c r="H2" s="10" t="s">
-        <v>77</v>
+        <v>165</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>26</v>
@@ -1168,7 +1174,7 @@
       </c>
       <c r="K2" s="11"/>
       <c r="N2" s="13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O2" s="13" t="s">
         <v>26</v>
@@ -1178,7 +1184,7 @@
       </c>
       <c r="Q2" s="14"/>
       <c r="T2" s="25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="U2" s="25" t="s">
         <v>26</v>
@@ -1188,7 +1194,7 @@
       </c>
       <c r="W2" s="26"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.75">
       <c r="A3" s="43"/>
       <c r="B3" s="3" t="s">
         <v>55</v>
@@ -1231,7 +1237,7 @@
       </c>
       <c r="W3" s="26"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.75">
       <c r="A4" s="43"/>
       <c r="B4" s="3" t="s">
         <v>56</v>
@@ -1263,7 +1269,7 @@
         <v>30</v>
       </c>
       <c r="Q4" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="T4" s="26" t="s">
         <v>56</v>
@@ -1276,7 +1282,7 @@
       </c>
       <c r="W4" s="26"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.75">
       <c r="A5" s="43"/>
       <c r="H5" s="11" t="s">
         <v>39</v>
@@ -1291,13 +1297,13 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.75">
       <c r="A6" s="43"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.75">
       <c r="A7" s="43"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.75">
       <c r="A8" s="43"/>
       <c r="B8" s="15" t="s">
         <v>71</v>
@@ -1310,7 +1316,7 @@
       </c>
       <c r="E8" s="15"/>
       <c r="H8" s="21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I8" s="21" t="s">
         <v>26</v>
@@ -1320,7 +1326,7 @@
       </c>
       <c r="K8" s="21"/>
       <c r="N8" s="8" t="s">
-        <v>83</v>
+        <v>166</v>
       </c>
       <c r="O8" s="8" t="s">
         <v>26</v>
@@ -1330,7 +1336,7 @@
       </c>
       <c r="Q8" s="8"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.75">
       <c r="A9" s="43"/>
       <c r="B9" s="16" t="s">
         <v>55</v>
@@ -1363,7 +1369,7 @@
       </c>
       <c r="Q9" s="9"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.75">
       <c r="A10" s="43"/>
       <c r="B10" s="16" t="s">
         <v>72</v>
@@ -1396,7 +1402,7 @@
       </c>
       <c r="Q10" s="9"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.75">
       <c r="A11" s="43"/>
       <c r="B11" s="16" t="s">
         <v>56</v>
@@ -1419,10 +1425,10 @@
       </c>
       <c r="K11" s="22"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.75">
       <c r="A12" s="43"/>
       <c r="B12" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>27</v>
@@ -1431,13 +1437,25 @@
         <v>34</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="I12" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="K12" s="50" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.75">
       <c r="A13" s="43"/>
       <c r="B13" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>28</v>
@@ -1446,36 +1464,36 @@
         <v>34</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.75">
       <c r="A14" s="43"/>
     </row>
-    <row r="15" spans="1:26" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" s="29" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A15" s="44"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.75">
       <c r="A16" s="45" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B16" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="H16" t="s">
+        <v>120</v>
+      </c>
+      <c r="N16" t="s">
         <v>121</v>
       </c>
-      <c r="H16" t="s">
+      <c r="T16" t="s">
         <v>122</v>
       </c>
-      <c r="N16" t="s">
+      <c r="Z16" t="s">
         <v>123</v>
       </c>
-      <c r="T16" t="s">
-        <v>124</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.75">
       <c r="A17" s="46"/>
       <c r="B17" s="4" t="s">
         <v>37</v>
@@ -1488,7 +1506,7 @@
       </c>
       <c r="E17" s="4"/>
       <c r="H17" s="23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I17" s="23" t="s">
         <v>26</v>
@@ -1498,7 +1516,7 @@
       </c>
       <c r="K17" s="23"/>
       <c r="N17" s="37" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O17" s="37" t="s">
         <v>26</v>
@@ -1508,7 +1526,7 @@
       </c>
       <c r="Q17" s="37"/>
       <c r="T17" s="35" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="U17" s="35" t="s">
         <v>26</v>
@@ -1518,7 +1536,7 @@
       </c>
       <c r="W17" s="35"/>
       <c r="Z17" s="39" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AA17" s="39" t="s">
         <v>26</v>
@@ -1528,7 +1546,7 @@
       </c>
       <c r="AC17" s="39"/>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.75">
       <c r="A18" s="46"/>
       <c r="B18" s="5" t="s">
         <v>5</v>
@@ -1581,7 +1599,7 @@
       </c>
       <c r="AC18" s="34"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.75">
       <c r="A19" s="46"/>
       <c r="B19" s="5" t="s">
         <v>39</v>
@@ -1593,40 +1611,40 @@
         <v>30</v>
       </c>
       <c r="E19" s="32" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G19" s="48" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="M19" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="N19" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="H19" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="I19" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="J19" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="K19" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="M19" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="N19" s="30" t="s">
+      <c r="O19" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="P19" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q19" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="O19" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="P19" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q19" s="38" t="s">
-        <v>105</v>
-      </c>
       <c r="T19" s="36" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="U19" s="36" t="s">
         <v>27</v>
@@ -1645,10 +1663,10 @@
         <v>30</v>
       </c>
       <c r="AC19" s="40" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.75">
       <c r="A20" s="46"/>
       <c r="B20" s="5" t="s">
         <v>40</v>
@@ -1660,11 +1678,11 @@
         <v>30</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G20" s="48"/>
       <c r="H20" s="24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I20" s="24" t="s">
         <v>28</v>
@@ -1673,11 +1691,11 @@
         <v>30</v>
       </c>
       <c r="K20" s="24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="M20" s="49"/>
       <c r="N20" s="30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O20" s="30" t="s">
         <v>28</v>
@@ -1687,10 +1705,10 @@
       </c>
       <c r="Q20" s="30"/>
       <c r="S20" s="35" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="T20" s="36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="U20" s="36" t="s">
         <v>28</v>
@@ -1699,10 +1717,10 @@
         <v>30</v>
       </c>
       <c r="W20" s="41" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="Z20" s="34" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AA20" s="34" t="s">
         <v>28</v>
@@ -1711,10 +1729,10 @@
         <v>30</v>
       </c>
       <c r="AC20" s="40" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.75">
       <c r="A21" s="46"/>
       <c r="B21" s="5" t="s">
         <v>38</v>
@@ -1728,7 +1746,7 @@
       <c r="E21" s="6"/>
       <c r="G21" s="48"/>
       <c r="H21" s="24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I21" s="24" t="s">
         <v>28</v>
@@ -1737,7 +1755,7 @@
         <v>30</v>
       </c>
       <c r="K21" s="24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="T21" s="36"/>
       <c r="U21" s="36"/>
@@ -1754,7 +1772,7 @@
       </c>
       <c r="AC21" s="34"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.75">
       <c r="A22" s="46"/>
       <c r="B22" s="5" t="s">
         <v>42</v>
@@ -1768,7 +1786,7 @@
       <c r="E22" s="5"/>
       <c r="G22" s="48"/>
       <c r="H22" s="24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I22" s="24" t="s">
         <v>28</v>
@@ -1777,7 +1795,7 @@
         <v>30</v>
       </c>
       <c r="K22" s="28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Z22" s="34" t="s">
         <v>36</v>
@@ -1790,7 +1808,7 @@
       </c>
       <c r="AC22" s="34"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.75">
       <c r="A23" s="46"/>
       <c r="B23" s="5" t="s">
         <v>67</v>
@@ -1803,7 +1821,7 @@
       </c>
       <c r="E23" s="5"/>
       <c r="H23" s="24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I23" s="24" t="s">
         <v>28</v>
@@ -1812,7 +1830,7 @@
         <v>30</v>
       </c>
       <c r="K23" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z23" s="34" t="s">
         <v>73</v>
@@ -1824,10 +1842,10 @@
         <v>31</v>
       </c>
       <c r="AC23" s="40" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.75">
       <c r="A24" s="46"/>
       <c r="B24" s="5" t="s">
         <v>41</v>
@@ -1842,7 +1860,7 @@
         <v>70</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I24" s="24" t="s">
         <v>28</v>
@@ -1851,10 +1869,10 @@
         <v>30</v>
       </c>
       <c r="K24" s="24" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.75">
       <c r="A25" s="46"/>
       <c r="B25" s="5" t="s">
         <v>66</v>
@@ -1869,7 +1887,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.75">
       <c r="A26" s="46"/>
       <c r="B26" s="5" t="s">
         <v>43</v>
@@ -1882,7 +1900,7 @@
       </c>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.75">
       <c r="A27" s="46"/>
       <c r="B27" s="7" t="s">
         <v>73</v>
@@ -1897,7 +1915,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.75">
       <c r="A28" s="46"/>
       <c r="B28" s="7" t="s">
         <v>75</v>
@@ -1906,16 +1924,16 @@
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.75">
       <c r="A29" s="46"/>
     </row>
-    <row r="30" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.75"/>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.75">
       <c r="A31" s="47" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.75">
       <c r="A32" s="47"/>
       <c r="B32" s="17" t="s">
         <v>20</v>
@@ -1928,7 +1946,7 @@
       </c>
       <c r="E32" s="17"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A33" s="47"/>
       <c r="B33" s="18" t="s">
         <v>5</v>
@@ -1943,7 +1961,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A34" s="47"/>
       <c r="B34" s="18" t="s">
         <v>7</v>
@@ -1956,7 +1974,7 @@
       </c>
       <c r="E34" s="18"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A35" s="47"/>
       <c r="B35" s="18" t="s">
         <v>8</v>
@@ -1971,7 +1989,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A36" s="47"/>
       <c r="B36" s="18" t="s">
         <v>9</v>
@@ -1986,7 +2004,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A37" s="47"/>
       <c r="B37" s="18" t="s">
         <v>10</v>
@@ -1999,7 +2017,7 @@
       </c>
       <c r="E37" s="18"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A38" s="47"/>
       <c r="B38" s="18" t="s">
         <v>12</v>
@@ -2012,7 +2030,7 @@
       </c>
       <c r="E38" s="18"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A39" s="47"/>
       <c r="B39" s="18" t="s">
         <v>11</v>
@@ -2027,7 +2045,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A40" s="47"/>
       <c r="B40" s="18" t="s">
         <v>44</v>
@@ -2040,7 +2058,7 @@
       </c>
       <c r="E40" s="18"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A41" s="47"/>
       <c r="B41" s="19" t="s">
         <v>32</v>
@@ -2053,7 +2071,7 @@
       </c>
       <c r="E41" s="18"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A42" s="47"/>
       <c r="B42" s="18" t="s">
         <v>36</v>
@@ -2066,7 +2084,7 @@
       </c>
       <c r="E42" s="18"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A43" s="47"/>
       <c r="B43" s="18" t="s">
         <v>13</v>
@@ -2081,7 +2099,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A44" s="47"/>
       <c r="B44" s="18" t="s">
         <v>14</v>
@@ -2096,7 +2114,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A45" s="47"/>
       <c r="B45" s="18" t="s">
         <v>15</v>
@@ -2109,7 +2127,7 @@
       </c>
       <c r="E45" s="18"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A46" s="47"/>
       <c r="B46" s="18" t="s">
         <v>16</v>
@@ -2122,7 +2140,7 @@
       </c>
       <c r="E46" s="18"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A47" s="47"/>
       <c r="B47" s="18" t="s">
         <v>35</v>
@@ -2135,7 +2153,7 @@
       </c>
       <c r="E47" s="18"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A48" s="47"/>
       <c r="B48" s="18" t="s">
         <v>49</v>
@@ -2150,7 +2168,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A49" s="47"/>
       <c r="B49" s="18" t="s">
         <v>17</v>
@@ -2165,7 +2183,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A50" s="47"/>
       <c r="B50" s="18" t="s">
         <v>23</v>
@@ -2180,7 +2198,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A51" s="47"/>
       <c r="B51" s="18" t="s">
         <v>24</v>
@@ -2195,7 +2213,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A52" s="47"/>
       <c r="B52" s="18" t="s">
         <v>25</v>
@@ -2210,7 +2228,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A53" s="47"/>
       <c r="B53" s="18" t="s">
         <v>18</v>
@@ -2225,7 +2243,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A54" s="47"/>
       <c r="B54" s="18" t="s">
         <v>19</v>
@@ -2240,10 +2258,10 @@
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A55" s="47"/>
       <c r="B55" s="18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>28</v>
@@ -2252,10 +2270,10 @@
         <v>34</v>
       </c>
       <c r="E55" s="33" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A56" s="47"/>
       <c r="B56" s="19" t="s">
         <v>21</v>
@@ -2270,7 +2288,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A57" s="47"/>
       <c r="B57" s="19" t="s">
         <v>46</v>
@@ -2283,7 +2301,7 @@
       </c>
       <c r="E57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A58" s="47"/>
       <c r="B58" s="19" t="s">
         <v>22</v>
@@ -2298,154 +2316,154 @@
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A59" s="47"/>
     </row>
-    <row r="60" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A60" s="47"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.75">
       <c r="B62" t="s">
+        <v>128</v>
+      </c>
+      <c r="E62" t="s">
+        <v>133</v>
+      </c>
+      <c r="H62" t="s">
+        <v>136</v>
+      </c>
+      <c r="K62" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="B63" t="s">
+        <v>129</v>
+      </c>
+      <c r="E63" t="s">
+        <v>129</v>
+      </c>
+      <c r="H63" t="s">
+        <v>137</v>
+      </c>
+      <c r="K63" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="B64" t="s">
         <v>130</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E64" t="s">
+        <v>83</v>
+      </c>
+      <c r="K64" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.75">
+      <c r="B65" t="s">
+        <v>131</v>
+      </c>
+      <c r="E65" t="s">
+        <v>134</v>
+      </c>
+      <c r="K65" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.75">
+      <c r="B66" t="s">
+        <v>102</v>
+      </c>
+      <c r="E66" t="s">
         <v>135</v>
       </c>
-      <c r="H62" t="s">
+      <c r="K66" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.75">
+      <c r="B67" t="s">
+        <v>132</v>
+      </c>
+      <c r="E67" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.75">
+      <c r="B71" t="s">
         <v>138</v>
       </c>
-      <c r="K62" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B63" t="s">
-        <v>131</v>
-      </c>
-      <c r="E63" t="s">
-        <v>131</v>
-      </c>
-      <c r="H63" t="s">
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.75">
+      <c r="B72" t="s">
         <v>139</v>
       </c>
-      <c r="K63" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B64" t="s">
-        <v>132</v>
-      </c>
-      <c r="E64" t="s">
-        <v>85</v>
-      </c>
-      <c r="K64" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B65" t="s">
-        <v>133</v>
-      </c>
-      <c r="E65" t="s">
-        <v>136</v>
-      </c>
-      <c r="K65" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B66" t="s">
-        <v>104</v>
-      </c>
-      <c r="E66" t="s">
-        <v>137</v>
-      </c>
-      <c r="K66" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B67" t="s">
-        <v>134</v>
-      </c>
-      <c r="E67" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B71" t="s">
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.75">
+      <c r="B73" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.75">
+      <c r="B74" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.75">
+      <c r="B75" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B72" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B73" t="s">
+    <row r="76" spans="2:11" x14ac:dyDescent="0.75">
+      <c r="B76" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.75">
+      <c r="B77" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.75">
+      <c r="B78" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.75">
+      <c r="B79" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B74" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B75" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B76" t="s">
+    <row r="80" spans="2:11" x14ac:dyDescent="0.75">
+      <c r="B80" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B77" t="s">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B81" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B78" t="s">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B82" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B79" t="s">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B83" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B80" t="s">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B84" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B81" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B82" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B83" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B84" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.75">
       <c r="B87" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C87" t="s">
         <v>26</v>
@@ -2454,7 +2472,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.75">
       <c r="B88" t="s">
         <v>55</v>
       </c>
@@ -2465,9 +2483,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.75">
       <c r="B89" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C89" t="s">
         <v>28</v>
@@ -2476,9 +2494,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.75">
       <c r="B90" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C90" t="s">
         <v>28</v>
@@ -2514,6 +2532,7 @@
     <hyperlink ref="AC23" location="configitem" display="foreingkey de configuração de itens"/>
     <hyperlink ref="W20" location="componentes" display="foreignkey de componentes"/>
     <hyperlink ref="E56" location="implementosX" display="foreignkey do arquivo de implementos especiais (betoneiras, bombas de concreto, munck etc.)"/>
+    <hyperlink ref="K12" location="modelos" display="foreignkey da tabela de modelos de veiculos e complementos"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>